<commit_message>
Parameters file modified to contain International recipe. StringsLocalization resource reduced Minor fixes to ParamStorage EA (Excessive Angle) defect commented out since it's not a requirement
</commit_message>
<xml_diff>
--- a/Documentation/Error map.xlsx
+++ b/Documentation/Error map.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\source\repos\PalletCheckWalmart\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\source\repos\PalletCheckWalmartRecipes\PalletCheckWalmart\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564FFC02-0151-4529-BBDA-F8BF08F8C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBA3242-C1C9-403F-80C0-B07412AF6D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0DE52C7B-7970-47B3-80ED-72FE7D59C4A1}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0DE52C7B-7970-47B3-80ED-72FE7D59C4A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="156">
   <si>
     <t>Defect Type</t>
   </si>
@@ -324,6 +325,189 @@
   </si>
   <si>
     <t>Side Nails protruding from Pallet</t>
+  </si>
+  <si>
+    <t>T_BN = 5,       // Top Board too Narrow</t>
+  </si>
+  <si>
+    <t>B_BN = 14,      // Bottom Board too Narrow</t>
+  </si>
+  <si>
+    <t>L_BPFP = 25,    // Left Block Protruding from Pallet</t>
+  </si>
+  <si>
+    <t>R_BPFP = 32,    // Right Block Protruding from Pallet</t>
+  </si>
+  <si>
+    <t>F_BPFP = 36,    // Front Block Protruding  from Pallet</t>
+  </si>
+  <si>
+    <t>B_BPFP = 42,    // Back Block Protruding  from Pallet</t>
+  </si>
+  <si>
+    <t>T_BW = 3,       // Top Broken Across Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B_BW = 12,      // Bottom Borken Across Width </t>
+  </si>
+  <si>
+    <t>L_EA = 23,      // Left Excesive Angle (Rotated Block)</t>
+  </si>
+  <si>
+    <t>R_EA = 30,      // Right Excesive Angle (Rotated Block)</t>
+  </si>
+  <si>
+    <t>F_EA = 35,      // Front Excessive Angle (Rotated Block)</t>
+  </si>
+  <si>
+    <t>B_EA = 41,      // Back Excessive Angle (Rotated Block)</t>
+  </si>
+  <si>
+    <t>T_ER = 9,       // Top Segmentation Error</t>
+  </si>
+  <si>
+    <t>B_ER = 18,      // Bottom Segmentation Error</t>
+  </si>
+  <si>
+    <t>L_FC = 26,      // Left Fork Clearance</t>
+  </si>
+  <si>
+    <t>R_FC = 33,      // Right Fork Clearance</t>
+  </si>
+  <si>
+    <t>F_FC = 39,      // Front Fork Clearance</t>
+  </si>
+  <si>
+    <t>B_FC = 45,      // Back Fork Clearance</t>
+  </si>
+  <si>
+    <t>T_MB = 8,       // Top Missing Board</t>
+  </si>
+  <si>
+    <t>B_MB = 17,      // Bottom Missing Board</t>
+  </si>
+  <si>
+    <t>L_MO = 21,      // Left Missing Block</t>
+  </si>
+  <si>
+    <t>R_MO = 28,      // Right Missing Block</t>
+  </si>
+  <si>
+    <t>F_MO = 37,      // Front Missing Block</t>
+  </si>
+  <si>
+    <t>B_MO = 43,      // Back Missing Block</t>
+  </si>
+  <si>
+    <t>T_MW = 4,       // Top Missing Wood</t>
+  </si>
+  <si>
+    <t>B_MW = 13,      // Bottom Missing Wood</t>
+  </si>
+  <si>
+    <t>L_MU = 22,      // Left Missing Chunk</t>
+  </si>
+  <si>
+    <t>R_MU = 29,      // Right Missing Chunk</t>
+  </si>
+  <si>
+    <t>F_MU = 38,      // Front Missing Chunks</t>
+  </si>
+  <si>
+    <t>B_MU = 44,      // Back Missing Chunks</t>
+  </si>
+  <si>
+    <t>T_MWA = 1,      // Top Missing Wood Across Lenght</t>
+  </si>
+  <si>
+    <t>L_MBMW // Left Middle Board Missing Wood</t>
+  </si>
+  <si>
+    <t>R_MBMW // Right Middle Board Missing Wood</t>
+  </si>
+  <si>
+    <t>T_PD = 6,       // Top Possbile Debris</t>
+  </si>
+  <si>
+    <t>B_PD = 15,      // Bottom Possible Debris</t>
+  </si>
+  <si>
+    <t>L_SNP = 20,     // Left Side Nail Protruding</t>
+  </si>
+  <si>
+    <t>R_SNP = 27,     // Right Side Nail Protruding</t>
+  </si>
+  <si>
+    <t>F_SNP = 34,     // Front Side Nail Protruding</t>
+  </si>
+  <si>
+    <t>B_SNP = 40,     // Back Side Nail Protruding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_RN = 2,       // Top Raised Nail              </t>
+  </si>
+  <si>
+    <t>B_RN = 11,      // Bottom Raised Nail</t>
+  </si>
+  <si>
+    <t>T_RNFC = 10,    // Top Raised Nail Fastener Cut off</t>
+  </si>
+  <si>
+    <t>B_RNFC = 19,    // Bottom Raised Nail Fastener Cut off</t>
+  </si>
+  <si>
+    <t>T_SH = 7,       // Top Board too Short</t>
+  </si>
+  <si>
+    <t>B_SH = 16,      // Bottom Board too Short</t>
+  </si>
+  <si>
+    <t>Board too Narrow</t>
+  </si>
+  <si>
+    <t>Broken Across Width</t>
+  </si>
+  <si>
+    <t>Segmentation Error</t>
+  </si>
+  <si>
+    <t>Missing Board</t>
+  </si>
+  <si>
+    <t>Missing Wood</t>
+  </si>
+  <si>
+    <t>Missing Wood Across Lenght</t>
+  </si>
+  <si>
+    <t>Possible Debris</t>
+  </si>
+  <si>
+    <t>Raised Nail</t>
+  </si>
+  <si>
+    <t>Board too Short</t>
+  </si>
+  <si>
+    <t>Block Protruding from Pallet</t>
+  </si>
+  <si>
+    <t>Excessive Angle</t>
+  </si>
+  <si>
+    <t>Missing Block</t>
+  </si>
+  <si>
+    <t>Missing Chunk</t>
+  </si>
+  <si>
+    <t>MBMW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNP </t>
+  </si>
+  <si>
+    <t>Side Nail Protruding</t>
   </si>
 </sst>
 </file>
@@ -363,12 +547,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -383,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -391,7 +587,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C5A30A-B25A-4A24-A650-5341B92F473D}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -984,7 +1181,7 @@
       <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" t="s">
         <v>86</v>
       </c>
       <c r="E19" t="s">
@@ -1041,12 +1238,12 @@
       <c r="B22" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D23" s="5" t="s">
+      <c r="D23" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1110,4 +1307,321 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB68E29-6DEB-4B67-9F55-E71FD883D563}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>